<commit_message>
Actualizados WBS y requisitos.
</commit_message>
<xml_diff>
--- a/doc/management/WBS.xlsx
+++ b/doc/management/WBS.xlsx
@@ -1,22 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28810"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Labora1\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ainhoazapirain/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11595"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15440" windowHeight="18000"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -24,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="37">
   <si>
     <t>1.1. Gestión de proyecto</t>
   </si>
@@ -105,6 +111,36 @@
   </si>
   <si>
     <t>REQUISITO</t>
+  </si>
+  <si>
+    <t>REQ_1, REQ_2</t>
+  </si>
+  <si>
+    <t>REQ_4</t>
+  </si>
+  <si>
+    <t>REQ_6</t>
+  </si>
+  <si>
+    <t>REQ_3, REQ_5</t>
+  </si>
+  <si>
+    <t>REQ_5</t>
+  </si>
+  <si>
+    <t>REQ_8</t>
+  </si>
+  <si>
+    <t>REQ_7</t>
+  </si>
+  <si>
+    <t>REQ_9</t>
+  </si>
+  <si>
+    <t>REQ_11</t>
+  </si>
+  <si>
+    <t>REQ_10</t>
   </si>
 </sst>
 </file>
@@ -482,25 +518,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" topLeftCell="D4" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="20" customWidth="1"/>
-    <col min="2" max="2" width="24.5703125" customWidth="1"/>
-    <col min="3" max="3" width="31.7109375" customWidth="1"/>
-    <col min="4" max="4" width="26.42578125" customWidth="1"/>
-    <col min="6" max="6" width="57.42578125" customWidth="1"/>
+    <col min="2" max="2" width="24.5" customWidth="1"/>
+    <col min="3" max="3" width="31.6640625" customWidth="1"/>
+    <col min="4" max="4" width="26.5" customWidth="1"/>
+    <col min="6" max="6" width="57.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="F1" s="7" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -509,7 +545,7 @@
       </c>
       <c r="F2" s="8"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="1"/>
       <c r="B3" t="s">
         <v>0</v>
@@ -518,7 +554,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C4" s="2" t="s">
         <v>1</v>
       </c>
@@ -526,7 +562,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C5" s="2" t="s">
         <v>2</v>
       </c>
@@ -534,7 +570,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C6" t="s">
         <v>3</v>
       </c>
@@ -542,7 +578,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C7" s="2" t="s">
         <v>4</v>
       </c>
@@ -550,7 +586,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C8" s="2" t="s">
         <v>5</v>
       </c>
@@ -558,7 +594,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
         <v>6</v>
       </c>
@@ -566,7 +602,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C10" s="2" t="s">
         <v>7</v>
       </c>
@@ -574,7 +610,7 @@
         <v>0.35</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C11" s="2"/>
       <c r="D11" t="s">
         <v>12</v>
@@ -582,8 +618,11 @@
       <c r="E11" s="5">
         <v>0.05</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F11" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C12" s="2"/>
       <c r="D12" t="s">
         <v>13</v>
@@ -591,8 +630,11 @@
       <c r="E12" s="5">
         <v>0.05</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F12" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C13" s="2"/>
       <c r="D13" t="s">
         <v>14</v>
@@ -600,40 +642,55 @@
       <c r="E13" s="5">
         <v>0.05</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F13" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="D14" t="s">
         <v>15</v>
       </c>
       <c r="E14" s="5">
         <v>0.05</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F14" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="D15" t="s">
         <v>16</v>
       </c>
       <c r="E15" s="5">
         <v>0.05</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F15" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="D16" t="s">
         <v>17</v>
       </c>
       <c r="E16" s="5">
         <v>0.05</v>
       </c>
-    </row>
-    <row r="17" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="F16" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="3:6" x14ac:dyDescent="0.2">
       <c r="D17" t="s">
         <v>18</v>
       </c>
       <c r="E17" s="5">
         <v>0.05</v>
       </c>
-    </row>
-    <row r="18" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="F17" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="18" spans="3:6" x14ac:dyDescent="0.2">
       <c r="C18" t="s">
         <v>8</v>
       </c>
@@ -641,31 +698,40 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="19" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:6" x14ac:dyDescent="0.2">
       <c r="D19" t="s">
         <v>19</v>
       </c>
       <c r="E19" s="5">
         <v>0.02</v>
       </c>
-    </row>
-    <row r="20" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="F19" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="20" spans="3:6" x14ac:dyDescent="0.2">
       <c r="D20" t="s">
         <v>20</v>
       </c>
       <c r="E20" s="5">
         <v>0.02</v>
       </c>
-    </row>
-    <row r="21" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="F20" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="21" spans="3:6" x14ac:dyDescent="0.2">
       <c r="D21" t="s">
         <v>21</v>
       </c>
       <c r="E21" s="5">
         <v>0.01</v>
       </c>
-    </row>
-    <row r="22" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="F21" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="22" spans="3:6" x14ac:dyDescent="0.2">
       <c r="C22" t="s">
         <v>9</v>
       </c>
@@ -673,23 +739,29 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="23" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:6" x14ac:dyDescent="0.2">
       <c r="D23" t="s">
         <v>22</v>
       </c>
       <c r="E23" s="5">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="24" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="F23" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="24" spans="3:6" x14ac:dyDescent="0.2">
       <c r="D24" t="s">
         <v>23</v>
       </c>
       <c r="E24" s="5">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="25" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="F24" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="25" spans="3:6" x14ac:dyDescent="0.2">
       <c r="C25" t="s">
         <v>10</v>
       </c>
@@ -697,7 +769,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="26" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:6" x14ac:dyDescent="0.2">
       <c r="C26" t="s">
         <v>25</v>
       </c>
@@ -706,6 +778,9 @@
       </c>
       <c r="E26" s="5">
         <v>0.3</v>
+      </c>
+      <c r="F26" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>